<commit_message>
Added vehicle size scenarios
</commit_message>
<xml_diff>
--- a/results/sensitivity_table.xlsx
+++ b/results/sensitivity_table.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Library/CloudStorage/Box-Box/BATMAN/Coding/Global_LIB_system/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A986CE-38FA-7E43-9370-336F3E190D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="18940" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -34,10 +40,10 @@
     <t>Faster electrification</t>
   </si>
   <si>
+    <t>Smaller batteries</t>
+  </si>
+  <si>
     <t>Replacements</t>
-  </si>
-  <si>
-    <t>Longer LIB lifetime</t>
   </si>
   <si>
     <t>Element</t>
@@ -76,8 +82,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,8 +113,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="53">
+  <fills count="55">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +166,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF8BAEC7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA9C1D4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -219,18 +238,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF7BA3C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA8C1D3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE8ECEF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFCEDAE4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -255,6 +274,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF7CA4C1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFDA3B46"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -285,7 +310,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF77A0BE"/>
+        <fgColor rgb="FF95B4CB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,6 +334,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF89ACC6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFE8A4A9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -333,7 +364,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD6E0E7"/>
+        <fgColor rgb="FF78A1BF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,7 +394,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD5DFE7"/>
+        <fgColor rgb="FF7AA2C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,12 +412,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF95B4CB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA2BDD1"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -399,7 +424,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF1E5E6"/>
+        <fgColor rgb="FF6F9BBB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,13 +436,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8BAEC7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFEAB0B5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA3BED2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,71 +471,83 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="17" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="18" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="19" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="20" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="21" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="22" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="23" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="24" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="25" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="26" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="27" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="28" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="29" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="30" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="31" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="32" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="33" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="34" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="35" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="36" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="37" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="38" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="39" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="40" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="41" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="42" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="43" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="44" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="45" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="46" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="47" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="48" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="49" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="50" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="51" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="52" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="53" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="54" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -557,7 +594,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -589,9 +626,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -623,6 +678,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -798,14 +871,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -834,294 +919,294 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2">
-        <v>-0.006960830257720274</v>
+        <v>-6.9608302577199611E-3</v>
       </c>
       <c r="C2" s="3">
-        <v>0.05653949654984509</v>
+        <v>5.6539496549845428E-2</v>
       </c>
       <c r="D2" s="4">
-        <v>0.2097017173870944</v>
+        <v>0.2097017173870947</v>
       </c>
       <c r="E2" s="5">
-        <v>-0.1892774944206156</v>
+        <v>-0.18927749442061539</v>
       </c>
       <c r="F2" s="6">
-        <v>-0.3873456052526047</v>
+        <v>-0.38734560525260459</v>
       </c>
       <c r="G2" s="7">
-        <v>0.6490911383742203</v>
+        <v>0.64909113837422105</v>
       </c>
       <c r="H2" s="8">
-        <v>-0.12988664960026</v>
+        <v>-0.26047650313153731</v>
       </c>
       <c r="I2" s="9">
-        <v>-0.2042956314763509</v>
+        <v>-0.1298866496002597</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="10">
-        <v>0.1117351185916075</v>
-      </c>
-      <c r="C3" s="11">
-        <v>-0.04487453600181238</v>
-      </c>
-      <c r="D3" s="12">
-        <v>-0.5705022799169602</v>
+      <c r="B3" s="11">
+        <v>0.11173511859160749</v>
+      </c>
+      <c r="C3" s="12">
+        <v>-4.4874536001812543E-2</v>
+      </c>
+      <c r="D3" s="13">
+        <v>-0.57050227991696023</v>
       </c>
       <c r="E3" s="5">
-        <v>-0.1893972006456307</v>
+        <v>-0.18939720064563079</v>
       </c>
       <c r="F3" s="6">
-        <v>-0.3865642990625577</v>
+        <v>-0.38656429906255779</v>
       </c>
       <c r="G3" s="7">
-        <v>0.6490767227586192</v>
+        <v>0.64907672275861916</v>
       </c>
       <c r="H3" s="8">
+        <v>-0.26090202715318589</v>
+      </c>
+      <c r="I3" s="9">
         <v>-0.1297528728782851</v>
       </c>
-      <c r="I3" s="9">
-        <v>-0.2038240010000014</v>
-      </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="13">
-        <v>0.2579837467383532</v>
-      </c>
-      <c r="C4" s="14">
-        <v>-0.1449723689223877</v>
-      </c>
-      <c r="D4" s="15">
+      <c r="B4" s="14">
+        <v>0.25798374673835339</v>
+      </c>
+      <c r="C4" s="15">
+        <v>-0.14497236892238771</v>
+      </c>
+      <c r="D4" s="16">
         <v>0.1271908837700772</v>
       </c>
-      <c r="E4" s="16">
-        <v>-0.2104258250090044</v>
-      </c>
-      <c r="F4" s="17">
-        <v>-0.3080751986619286</v>
-      </c>
-      <c r="G4" s="18">
-        <v>0.4546609280590591</v>
-      </c>
-      <c r="H4" s="19">
+      <c r="E4" s="17">
+        <v>-0.21042582500900439</v>
+      </c>
+      <c r="F4" s="18">
+        <v>-0.30807519866192862</v>
+      </c>
+      <c r="G4" s="19">
+        <v>0.45466092805905961</v>
+      </c>
+      <c r="H4" s="20">
+        <v>-0.33231148087292739</v>
+      </c>
+      <c r="I4" s="21">
         <v>-0.134723986825321</v>
       </c>
-      <c r="I4" s="20">
-        <v>0.1591327482139264</v>
-      </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="21">
-        <v>0.04174559093251962</v>
-      </c>
-      <c r="C5" s="22">
-        <v>-0.03005137290875014</v>
-      </c>
-      <c r="D5" s="17">
-        <v>-0.3112084841611832</v>
-      </c>
-      <c r="E5" s="9">
-        <v>-0.204633805112181</v>
-      </c>
-      <c r="F5" s="23">
-        <v>-0.2480728768017632</v>
-      </c>
-      <c r="G5" s="24">
-        <v>0.5083608797802019</v>
-      </c>
-      <c r="H5" s="19">
-        <v>-0.1334228684473429</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.05982199455232769</v>
+      <c r="B5" s="22">
+        <v>4.1745590932519408E-2</v>
+      </c>
+      <c r="C5" s="23">
+        <v>-3.0051372908750141E-2</v>
+      </c>
+      <c r="D5" s="18">
+        <v>-0.3112084841611833</v>
+      </c>
+      <c r="E5" s="10">
+        <v>-0.20463380511218091</v>
+      </c>
+      <c r="F5" s="24">
+        <v>-0.2480728768017634</v>
+      </c>
+      <c r="G5" s="25">
+        <v>0.50836087978020228</v>
+      </c>
+      <c r="H5" s="26">
+        <v>-0.32528774637520919</v>
+      </c>
+      <c r="I5" s="21">
+        <v>-0.13342286844734291</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="25">
-        <v>1.551833437472984</v>
-      </c>
-      <c r="C6" s="26">
-        <v>-0.902429783518186</v>
-      </c>
-      <c r="D6" s="26">
-        <v>-0.9444746874495324</v>
-      </c>
-      <c r="E6" s="27">
-        <v>-0.1808294882051173</v>
-      </c>
-      <c r="F6" s="28">
-        <v>-0.4880494140901102</v>
-      </c>
-      <c r="G6" s="29">
-        <v>0.7258876152271854</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="B6" s="27">
+        <v>1.5518334374729841</v>
+      </c>
+      <c r="C6" s="28">
+        <v>-0.90242978351818603</v>
+      </c>
+      <c r="D6" s="28">
+        <v>-0.94447468744953245</v>
+      </c>
+      <c r="E6" s="29">
+        <v>-0.18082948820511729</v>
+      </c>
+      <c r="F6" s="30">
+        <v>-0.48804941409011021</v>
+      </c>
+      <c r="G6" s="31">
+        <v>0.72588761522718537</v>
+      </c>
+      <c r="H6" s="32">
+        <v>-0.21660007192402109</v>
+      </c>
+      <c r="I6" s="9">
         <v>-0.1278342213017099</v>
       </c>
-      <c r="I6" s="30">
-        <v>-0.3502614842518006</v>
-      </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="31">
-        <v>-0.03645220429724872</v>
-      </c>
-      <c r="C7" s="25">
+      <c r="B7" s="33">
+        <v>-3.6452204297248707E-2</v>
+      </c>
+      <c r="C7" s="27">
         <v>1.350378087213767</v>
       </c>
-      <c r="D7" s="32">
-        <v>0.02097818100680924</v>
+      <c r="D7" s="34">
+        <v>2.0978181006809239E-2</v>
       </c>
       <c r="E7" s="5">
-        <v>-0.1913468024388049</v>
+        <v>-0.191346802438805</v>
       </c>
       <c r="F7" s="6">
-        <v>-0.3854066187078174</v>
-      </c>
-      <c r="G7" s="33">
-        <v>0.6175834999241238</v>
-      </c>
-      <c r="H7" s="19">
-        <v>-0.1350530265049626</v>
-      </c>
-      <c r="I7" s="14">
-        <v>-0.1475829976224533</v>
+        <v>-0.38540661870781739</v>
+      </c>
+      <c r="G7" s="35">
+        <v>0.61758349992412354</v>
+      </c>
+      <c r="H7" s="36">
+        <v>-0.27355815117537768</v>
+      </c>
+      <c r="I7" s="21">
+        <v>-0.1350530265049627</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="6">
-        <v>-0.3861774744787444</v>
-      </c>
-      <c r="C8" s="34">
-        <v>0.5395793137434403</v>
-      </c>
-      <c r="D8" s="35">
-        <v>-0.4834799290151884</v>
-      </c>
-      <c r="E8" s="16">
-        <v>-0.2067901042315005</v>
-      </c>
-      <c r="F8" s="36">
-        <v>-0.1183739870946168</v>
-      </c>
-      <c r="G8" s="37">
-        <v>0.503453764536154</v>
-      </c>
-      <c r="H8" s="19">
-        <v>-0.1366377673986283</v>
-      </c>
-      <c r="I8" s="38">
-        <v>0.08081684492433408</v>
+        <v>-0.38617747447874418</v>
+      </c>
+      <c r="C8" s="37">
+        <v>0.5395793137434407</v>
+      </c>
+      <c r="D8" s="38">
+        <v>-0.48347992901518821</v>
+      </c>
+      <c r="E8" s="17">
+        <v>-0.20679010423150049</v>
+      </c>
+      <c r="F8" s="39">
+        <v>-0.11837398709461661</v>
+      </c>
+      <c r="G8" s="40">
+        <v>0.50345376453615442</v>
+      </c>
+      <c r="H8" s="41">
+        <v>-0.34818599726838051</v>
+      </c>
+      <c r="I8" s="21">
+        <v>-0.13663776739862801</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="39">
-        <v>-0.5057937090587652</v>
-      </c>
-      <c r="C9" s="40">
+      <c r="B9" s="42">
+        <v>-0.50579370905876531</v>
+      </c>
+      <c r="C9" s="43">
         <v>0.2298731397608422</v>
       </c>
-      <c r="D9" s="41">
-        <v>-0.4749369704205066</v>
-      </c>
-      <c r="E9" s="9">
-        <v>-0.2050383162112901</v>
-      </c>
-      <c r="F9" s="42">
-        <v>-0.1102846424598815</v>
-      </c>
-      <c r="G9" s="37">
-        <v>0.5015547482321628</v>
-      </c>
-      <c r="H9" s="19">
-        <v>-0.1327677684551017</v>
-      </c>
-      <c r="I9" s="43">
-        <v>0.07073986443784726</v>
+      <c r="D9" s="44">
+        <v>-0.4749369704205067</v>
+      </c>
+      <c r="E9" s="10">
+        <v>-0.2050383162112904</v>
+      </c>
+      <c r="F9" s="45">
+        <v>-0.110284642459882</v>
+      </c>
+      <c r="G9" s="40">
+        <v>0.50155474823216262</v>
+      </c>
+      <c r="H9" s="46">
+        <v>-0.34297603635267898</v>
+      </c>
+      <c r="I9" s="21">
+        <v>-0.1327677684551018</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="4">
-        <v>0.2081256549208945</v>
-      </c>
-      <c r="C10" s="44">
-        <v>-0.09557683260033555</v>
-      </c>
-      <c r="D10" s="45">
-        <v>-0.4314930204270776</v>
-      </c>
-      <c r="E10" s="46">
-        <v>-0.2159893056068384</v>
-      </c>
-      <c r="F10" s="47">
-        <v>-0.1603800747096561</v>
-      </c>
-      <c r="G10" s="48">
-        <v>0.4056678832321395</v>
-      </c>
-      <c r="H10" s="19">
+        <v>0.20812565492089419</v>
+      </c>
+      <c r="C10" s="47">
+        <v>-9.5576832600335115E-2</v>
+      </c>
+      <c r="D10" s="48">
+        <v>-0.43149302042707782</v>
+      </c>
+      <c r="E10" s="32">
+        <v>-0.2159893056068381</v>
+      </c>
+      <c r="F10" s="49">
+        <v>-0.1603800747096564</v>
+      </c>
+      <c r="G10" s="50">
+        <v>0.40566788323214009</v>
+      </c>
+      <c r="H10" s="51">
+        <v>-0.3889647495743262</v>
+      </c>
+      <c r="I10" s="21">
         <v>-0.1360371216390745</v>
       </c>
-      <c r="I10" s="49">
-        <v>0.2558447228666417</v>
-      </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="50">
-        <v>0.4748174870649992</v>
-      </c>
-      <c r="C11" s="51">
-        <v>-0.2613333578392641</v>
-      </c>
-      <c r="D11" s="52">
-        <v>0.4870483785022315</v>
-      </c>
-      <c r="E11" s="27">
+      <c r="B11" s="52">
+        <v>0.47481748706499921</v>
+      </c>
+      <c r="C11" s="8">
+        <v>-0.26133335783926409</v>
+      </c>
+      <c r="D11" s="53">
+        <v>0.48704837850223193</v>
+      </c>
+      <c r="E11" s="29">
         <v>-0.1808503364837051</v>
       </c>
-      <c r="F11" s="26">
-        <v>-0.6081559131806864</v>
-      </c>
-      <c r="G11" s="29">
-        <v>0.7262014591772497</v>
-      </c>
-      <c r="H11" s="8">
-        <v>-0.1278379947775811</v>
-      </c>
-      <c r="I11" s="30">
-        <v>-0.350273861878256</v>
+      <c r="F11" s="28">
+        <v>-0.60815591318068662</v>
+      </c>
+      <c r="G11" s="31">
+        <v>0.72620145917724965</v>
+      </c>
+      <c r="H11" s="54">
+        <v>-0.15224196724472319</v>
+      </c>
+      <c r="I11" s="9">
+        <v>-0.12783799477758109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added size scenarios to case6
</commit_message>
<xml_diff>
--- a/results/sensitivity_table.xlsx
+++ b/results/sensitivity_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Library/CloudStorage/Box-Box/BATMAN/Coding/Global_LIB_system/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A986CE-38FA-7E43-9370-336F3E190D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1260C6E-270F-9843-AEF1-B9ECCBAD7307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="18940" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -872,21 +872,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1209,6 +1209,36 @@
         <v>-0.12783799477758109</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="26"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="32"/>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="36"/>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="41"/>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="46"/>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="51"/>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="54"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Re-did Figures and ran all updated scenarios
</commit_message>
<xml_diff>
--- a/results/sensitivity_table.xlsx
+++ b/results/sensitivity_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Library/CloudStorage/Box-Box/BATMAN/Coding/Global_LIB_system/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD6A3E5-BE8C-194A-9B9B-02A2240FADC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8824599-815C-7B4D-9C86-E35D5786F336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12760" yWindow="1640" windowWidth="26880" windowHeight="20720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="32860" windowHeight="27740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,9 @@
     <t>Shift to Next generation chemistries</t>
   </si>
   <si>
+    <t>Efficient recycling</t>
+  </si>
+  <si>
     <t>Faster electrification</t>
   </si>
   <si>
@@ -71,9 +74,6 @@
   </si>
   <si>
     <t>Fleet growth reduction</t>
-  </si>
-  <si>
-    <t>Direct recycling</t>
   </si>
   <si>
     <t>Replacements and reuse</t>
@@ -121,7 +121,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="52">
+  <fills count="51">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +148,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC0D7C4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFB4D1BA"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -220,6 +226,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFB6D2BB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFE37B83"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -310,7 +322,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA3C6AB"/>
+        <fgColor rgb="FFC1D8C6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5C7AC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,13 +358,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF88B691"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFAACBB1"/>
+        <fgColor rgb="FF89B793"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBBD5C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -358,12 +376,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC1D8C6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFE3EDE4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -388,13 +400,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFACCCB2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC0D7C4"/>
+        <fgColor rgb="FFDEEAE1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,18 +413,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBDD6C2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE27880"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDEEAE1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,7 +451,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -466,8 +460,8 @@
     <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -477,29 +471,29 @@
     <xf numFmtId="9" fontId="2" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="17" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="17" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="18" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="19" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="19" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="20" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="21" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="22" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="23" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="23" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="24" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="3" fillId="25" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="26" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="27" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="26" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="27" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="3" fillId="28" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="29" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="30" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="30" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="31" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="32" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="33" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="33" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="34" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="35" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="3" fillId="36" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="37" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="37" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="38" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="39" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="39" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="40" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="41" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="42" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -509,9 +503,8 @@
     <xf numFmtId="9" fontId="2" fillId="46" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="47" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="48" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="49" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="49" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="50" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="51" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,22 +846,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -880,310 +866,310 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
-        <v>-8.4764025385328911E-3</v>
+        <v>-8.4751261579213942E-3</v>
       </c>
       <c r="C2" s="3">
-        <v>6.0653568506901949E-2</v>
+        <v>6.0657231593944948E-2</v>
       </c>
       <c r="D2" s="4">
-        <v>0.1539551810440549</v>
+        <v>0.1539316159231463</v>
       </c>
       <c r="E2" s="5">
-        <v>-0.31529202102389509</v>
-      </c>
-      <c r="F2" s="5">
-        <v>-0.31967010749122382</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0.68530976008387634</v>
-      </c>
-      <c r="H2" s="7">
-        <v>-0.19407347844348991</v>
-      </c>
-      <c r="I2" s="8">
-        <v>-0.17459169727591781</v>
-      </c>
-      <c r="J2" s="9">
-        <v>-7.2663449898193316E-2</v>
+        <v>-0.2559501827093828</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.68317007917896733</v>
+      </c>
+      <c r="G2" s="8">
+        <v>-0.1940305738344083</v>
+      </c>
+      <c r="H2" s="10">
+        <v>-7.2650744958657476E-2</v>
+      </c>
+      <c r="I2" s="9">
+        <v>-0.1745678460277042</v>
+      </c>
+      <c r="J2" s="6">
+        <v>-0.31925215899559678</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="10">
-        <v>0.1093674279484768</v>
-      </c>
-      <c r="C3" s="11">
-        <v>-3.3933624829083867E-2</v>
-      </c>
-      <c r="D3" s="12">
-        <v>-0.48244062766453311</v>
+        <v>9</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.1093704973747313</v>
+      </c>
+      <c r="C3" s="12">
+        <v>-3.3924990236269187E-2</v>
+      </c>
+      <c r="D3" s="13">
+        <v>-0.48235335927645961</v>
       </c>
       <c r="E3" s="5">
-        <v>-0.31504240033345238</v>
-      </c>
-      <c r="F3" s="13">
-        <v>-0.30436698139871821</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0.68623285410884316</v>
-      </c>
-      <c r="H3" s="7">
-        <v>-0.19469818379976661</v>
-      </c>
-      <c r="I3" s="8">
-        <v>-0.17506983011080651</v>
-      </c>
-      <c r="J3" s="9">
-        <v>-7.28922513468898E-2</v>
+        <v>-0.25630890911638732</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.68409551365128962</v>
+      </c>
+      <c r="G3" s="8">
+        <v>-0.1946557210978884</v>
+      </c>
+      <c r="H3" s="10">
+        <v>-7.2879664625512028E-2</v>
+      </c>
+      <c r="I3" s="9">
+        <v>-0.1750462106294394</v>
+      </c>
+      <c r="J3" s="14">
+        <v>-0.3039699706686611</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="14">
-        <v>0.24063992171326209</v>
-      </c>
-      <c r="C4" s="15">
-        <v>-0.1220283157727927</v>
-      </c>
-      <c r="D4" s="16">
-        <v>6.3153355473825154E-2</v>
+        <v>10</v>
+      </c>
+      <c r="B4" s="15">
+        <v>0.24064161346987351</v>
+      </c>
+      <c r="C4" s="16">
+        <v>-0.12202910789826101</v>
+      </c>
+      <c r="D4" s="17">
+        <v>6.3166072856821506E-2</v>
       </c>
       <c r="E4" s="5">
-        <v>-0.31317053018891361</v>
-      </c>
-      <c r="F4" s="5">
-        <v>-0.3126698942297168</v>
-      </c>
-      <c r="G4" s="17">
-        <v>0.64375848065802055</v>
-      </c>
-      <c r="H4" s="18">
-        <v>-0.16846138682328629</v>
-      </c>
-      <c r="I4" s="8">
-        <v>-0.17513898011519241</v>
-      </c>
-      <c r="J4" s="9">
-        <v>-7.2932395370613107E-2</v>
+        <v>-0.25612475770691939</v>
+      </c>
+      <c r="F4" s="19">
+        <v>0.64174402641294492</v>
+      </c>
+      <c r="G4" s="20">
+        <v>-0.16843197081126349</v>
+      </c>
+      <c r="H4" s="10">
+        <v>-7.29199872829909E-2</v>
+      </c>
+      <c r="I4" s="9">
+        <v>-0.17511566844079621</v>
+      </c>
+      <c r="J4" s="18">
+        <v>-0.31227514517779242</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="19">
-        <v>4.164595155812114E-2</v>
-      </c>
-      <c r="C5" s="20">
-        <v>-4.5989633195172672E-2</v>
-      </c>
-      <c r="D5" s="21">
-        <v>-0.22750474389609701</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="21">
+        <v>4.163865199372592E-2</v>
+      </c>
+      <c r="C5" s="22">
+        <v>-4.5998054744482209E-2</v>
+      </c>
+      <c r="D5" s="23">
+        <v>-0.22745882355489661</v>
       </c>
       <c r="E5" s="5">
-        <v>-0.31437326701750767</v>
-      </c>
-      <c r="F5" s="22">
-        <v>-0.35857412623999851</v>
-      </c>
-      <c r="G5" s="23">
-        <v>0.66632457983816185</v>
-      </c>
-      <c r="H5" s="24">
-        <v>-0.1824510608514566</v>
-      </c>
-      <c r="I5" s="8">
-        <v>-0.17493117968650751</v>
-      </c>
-      <c r="J5" s="9">
-        <v>-7.2824509989285732E-2</v>
+        <v>-0.25613796117870269</v>
+      </c>
+      <c r="F5" s="25">
+        <v>0.66424209450532401</v>
+      </c>
+      <c r="G5" s="26">
+        <v>-0.18241470799602791</v>
+      </c>
+      <c r="H5" s="10">
+        <v>-7.281187107933218E-2</v>
+      </c>
+      <c r="I5" s="9">
+        <v>-0.17490742153324701</v>
+      </c>
+      <c r="J5" s="24">
+        <v>-0.35811256517289569</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="25">
-        <v>1.5385269479023831</v>
-      </c>
-      <c r="C6" s="26">
-        <v>-0.89652498338433406</v>
-      </c>
-      <c r="D6" s="12">
-        <v>-0.48138881956587021</v>
+        <v>12</v>
+      </c>
+      <c r="B6" s="27">
+        <v>1.538500155703022</v>
+      </c>
+      <c r="C6" s="28">
+        <v>-0.89652432095241419</v>
+      </c>
+      <c r="D6" s="13">
+        <v>-0.4813008851334446</v>
       </c>
       <c r="E6" s="5">
-        <v>-0.31545828516140939</v>
-      </c>
-      <c r="F6" s="27">
-        <v>-0.1567546319980318</v>
-      </c>
-      <c r="G6" s="28">
-        <v>0.69114219929609966</v>
-      </c>
-      <c r="H6" s="29">
-        <v>-0.19636431987052549</v>
-      </c>
-      <c r="I6" s="8">
-        <v>-0.17474910892933621</v>
-      </c>
-      <c r="J6" s="9">
-        <v>-7.2740484962590307E-2</v>
+        <v>-0.25609409725950832</v>
+      </c>
+      <c r="F6" s="30">
+        <v>0.68898721121791873</v>
+      </c>
+      <c r="G6" s="31">
+        <v>-0.1963187962922418</v>
+      </c>
+      <c r="H6" s="10">
+        <v>-7.2727807734374345E-2</v>
+      </c>
+      <c r="I6" s="9">
+        <v>-0.1747253145815767</v>
+      </c>
+      <c r="J6" s="29">
+        <v>-0.15654900652731771</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="30">
-        <v>-2.9127234671772629E-2</v>
-      </c>
-      <c r="C7" s="25">
-        <v>1.2902873250224669</v>
-      </c>
-      <c r="D7" s="31">
-        <v>-0.44737071452706889</v>
-      </c>
-      <c r="E7" s="5">
-        <v>-0.31832491441730298</v>
-      </c>
-      <c r="F7" s="32">
-        <v>-0.40626608180759333</v>
-      </c>
-      <c r="G7" s="33">
-        <v>0.65198545751685177</v>
-      </c>
-      <c r="H7" s="24">
-        <v>-0.18011404632239311</v>
-      </c>
-      <c r="I7" s="18">
-        <v>-0.1646768572169969</v>
-      </c>
-      <c r="J7" s="34">
-        <v>-6.7974154151638405E-2</v>
+        <v>13</v>
+      </c>
+      <c r="B7" s="32">
+        <v>-2.9123840084106071E-2</v>
+      </c>
+      <c r="C7" s="27">
+        <v>1.2902699198629211</v>
+      </c>
+      <c r="D7" s="33">
+        <v>-0.44727232407173528</v>
+      </c>
+      <c r="E7" s="34">
+        <v>-0.2478972509969106</v>
+      </c>
+      <c r="F7" s="36">
+        <v>0.64985673215043382</v>
+      </c>
+      <c r="G7" s="26">
+        <v>-0.1800675705589164</v>
+      </c>
+      <c r="H7" s="37">
+        <v>-6.7960317700573147E-2</v>
+      </c>
+      <c r="I7" s="20">
+        <v>-0.16465102918402741</v>
+      </c>
+      <c r="J7" s="35">
+        <v>-0.40571985023372731</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="35">
-        <v>-0.34091431548696077</v>
-      </c>
-      <c r="C8" s="36">
-        <v>0.5974760365183438</v>
-      </c>
-      <c r="D8" s="37">
-        <v>-0.5548636992021535</v>
-      </c>
-      <c r="E8" s="38">
-        <v>-0.37170951919995487</v>
-      </c>
-      <c r="F8" s="39">
-        <v>-9.1563489882487997E-2</v>
-      </c>
-      <c r="G8" s="28">
-        <v>0.6879927139597205</v>
-      </c>
-      <c r="H8" s="40">
-        <v>-0.24942043089554089</v>
-      </c>
-      <c r="I8" s="41">
-        <v>-6.1483057467036827E-2</v>
+        <v>14</v>
+      </c>
+      <c r="B8" s="38">
+        <v>-0.34079813359373029</v>
+      </c>
+      <c r="C8" s="39">
+        <v>0.59763755979223598</v>
+      </c>
+      <c r="D8" s="40">
+        <v>-0.5545716392559551</v>
+      </c>
+      <c r="E8" s="41">
+        <v>-0.28050043888496318</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.68485914890134147</v>
+      </c>
+      <c r="G8" s="34">
+        <v>-0.2492431815204281</v>
+      </c>
+      <c r="H8" s="44">
+        <v>2.2455020739639359E-2</v>
+      </c>
+      <c r="I8" s="43">
+        <v>-6.1659247690291977E-2</v>
       </c>
       <c r="J8" s="42">
-        <v>2.2616367281670529E-2</v>
+        <v>-9.1387847352241217E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="43">
-        <v>-0.49801287740802758</v>
-      </c>
-      <c r="C9" s="44">
-        <v>0.22127729857048159</v>
-      </c>
-      <c r="D9" s="12">
-        <v>-0.48243257578691751</v>
-      </c>
-      <c r="E9" s="45">
-        <v>-0.3643242181047569</v>
-      </c>
-      <c r="F9" s="39">
-        <v>-8.606331750661915E-2</v>
-      </c>
-      <c r="G9" s="28">
-        <v>0.69168374359090468</v>
-      </c>
-      <c r="H9" s="46">
-        <v>-0.25122817068603909</v>
-      </c>
-      <c r="I9" s="41">
-        <v>-6.2012168174179122E-2</v>
-      </c>
-      <c r="J9" s="42">
-        <v>2.2800972794348728E-2</v>
+        <v>15</v>
+      </c>
+      <c r="B9" s="45">
+        <v>-0.49798997258244748</v>
+      </c>
+      <c r="C9" s="46">
+        <v>0.22126027092746409</v>
+      </c>
+      <c r="D9" s="13">
+        <v>-0.48220368536315222</v>
+      </c>
+      <c r="E9" s="41">
+        <v>-0.2810717298130756</v>
+      </c>
+      <c r="F9" s="30">
+        <v>0.68861584841945067</v>
+      </c>
+      <c r="G9" s="5">
+        <v>-0.25106358271826729</v>
+      </c>
+      <c r="H9" s="44">
+        <v>2.2639998320184949E-2</v>
+      </c>
+      <c r="I9" s="43">
+        <v>-6.2190313524520743E-2</v>
+      </c>
+      <c r="J9" s="47">
+        <v>-8.5902824406754716E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="47">
-        <v>0.2424683753429161</v>
-      </c>
-      <c r="C10" s="15">
-        <v>-0.1175863548612906</v>
-      </c>
-      <c r="D10" s="48">
-        <v>-0.26778692652326441</v>
-      </c>
-      <c r="E10" s="22">
-        <v>-0.35711888005489878</v>
-      </c>
-      <c r="F10" s="9">
-        <v>-7.3414527143797148E-2</v>
-      </c>
-      <c r="G10" s="49">
-        <v>0.65879030688961104</v>
-      </c>
-      <c r="H10" s="21">
-        <v>-0.2308942323494611</v>
-      </c>
-      <c r="I10" s="50">
-        <v>-7.843656426505119E-2</v>
-      </c>
-      <c r="J10" s="51">
-        <v>9.2876217686719258E-3</v>
+        <v>16</v>
+      </c>
+      <c r="B10" s="48">
+        <v>0.24236548634270599</v>
+      </c>
+      <c r="C10" s="16">
+        <v>-0.11751601352071871</v>
+      </c>
+      <c r="D10" s="49">
+        <v>-0.26766228462197877</v>
+      </c>
+      <c r="E10" s="41">
+        <v>-0.27778287488945902</v>
+      </c>
+      <c r="F10" s="36">
+        <v>0.65596758507301667</v>
+      </c>
+      <c r="G10" s="23">
+        <v>-0.23076550527165379</v>
+      </c>
+      <c r="H10" s="50">
+        <v>9.16079073812902E-3</v>
+      </c>
+      <c r="I10" s="47">
+        <v>-7.8573590274764446E-2</v>
+      </c>
+      <c r="J10" s="10">
+        <v>-7.3285855025087693E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>